<commit_message>
changed way of filling data table in document
</commit_message>
<xml_diff>
--- a/src/main/resources/example/plan_template.xlsx
+++ b/src/main/resources/example/plan_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xyz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\planner\src\main\resources\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F9EAD3-0418-46AB-B570-58F355B00F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E66F4C3D-12CB-4182-BDEE-197338A2E33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9060" tabRatio="791" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="9060" tabRatio="791" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general info" sheetId="2" r:id="rId1"/>
@@ -206,9 +206,6 @@
     <t>Day 2: Back</t>
   </si>
   <si>
-    <t>Day 3: popo</t>
-  </si>
-  <si>
     <t>Day 4: Chest and Calves</t>
   </si>
   <si>
@@ -227,22 +224,25 @@
     <t>Lorem ipsum ĄĆĘÓŁŃŻŹąćęółńżź sit amet consectetur adipisicing elit. Maxime mollitia, molestiae quas vel sint commodi repudiandae&lt;br&gt;&lt;br&gt; consequuntur voluptatum. Dfgash njgadisug jdsngidahsigu ndsjf adfn iabni b bnai biu b i abiabdfhi i bdbbdasi bi iab fbi ij biadbiabi ijabd i &lt;br&gt;KKKAAKAKAKAkkakakakka</t>
   </si>
   <si>
-    <t>Day 1: Chicken ĄĆĘÓŁŃŻŹąćęółńżź ĄĆĘÓŁŃŻŹąćęółńżź</t>
-  </si>
-  <si>
     <t>ĄĆĘÓŁŃŻŹąćęółńżź @https://www.youtube.com/watch?v=6iFbuIpe68k</t>
   </si>
   <si>
     <t>TRAINING NAME&lt;br&gt;ĄĆĘÓŁŃŻŹąćęółńżź</t>
   </si>
   <si>
-    <t>xyz</t>
-  </si>
-  <si>
     <t>excercise 3 sadfasfasfasfasfasfsafsd sadfasd dafadsf asdfasdf saa asfasfa</t>
   </si>
   <si>
     <t>excercise 2 @https://www.youtube.com/watch?v=6iFbuIpe68k</t>
+  </si>
+  <si>
+    <t>Xyz</t>
+  </si>
+  <si>
+    <t>Day 1: Legs ĄĆĘÓŁŃŻŹąćęółńżź ĄĆĘÓŁŃŻŹąćęółńżź</t>
+  </si>
+  <si>
+    <t>Day 3: ABS and arms</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
         <v>49</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -600,7 +600,7 @@
         <v>48</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -613,9 +613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E41196D1-A9F4-4135-A83A-0AE692634E19}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:C13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -637,7 +635,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -675,9 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -689,12 +685,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>39</v>
@@ -714,7 +710,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -728,7 +724,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>13</v>
@@ -742,7 +738,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>5</v>
@@ -753,7 +749,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -765,12 +761,12 @@
         <v>17</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
@@ -793,7 +789,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.77734375" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="10.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
@@ -904,9 +900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B153C0B5-E6E6-4A38-AE69-25CE7D0B1AB6}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -916,7 +910,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -940,7 +934,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
@@ -954,7 +948,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>5</v>
@@ -987,7 +981,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>